<commit_message>
adding minor changes to mpd_lr_stats_subplots.py and images and statistical results regarding 2nd preliminary experiment
</commit_message>
<xml_diff>
--- a/code/MPD/results/statistics/MPD_MPD_mean.xlsx
+++ b/code/MPD/results/statistics/MPD_MPD_mean.xlsx
@@ -612,7 +612,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FlairFast_MCC scores</t>
+          <t>Flair Fast_MCC scores</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -636,7 +636,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>FlairFast_Classification time</t>
+          <t>Flair Fast_Classification time</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -660,7 +660,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>FlairFast_Training time</t>
+          <t>Flair Fast_Training time</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -900,7 +900,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Bert_smix_MCC scores</t>
+          <t>BertS_MCC scores</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -924,7 +924,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Bert_smix_Classification time</t>
+          <t>BertS_Classification time</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -948,7 +948,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Bert_smix_Training time</t>
+          <t>BertS_Training time</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1044,7 +1044,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>XLNet_smix_MCC scores</t>
+          <t>XLNetS_MCC scores</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1068,7 +1068,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>XLNet_smix_Classification time</t>
+          <t>XLNetS_Classification time</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1092,7 +1092,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>XLNet_smix_Training time</t>
+          <t>XLNetS_Training time</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1188,7 +1188,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Roberta_L_MCC scores</t>
+          <t>RobertaL_MCC scores</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1212,7 +1212,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Roberta_L_Classification time</t>
+          <t>RobertaL_Classification time</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1236,7 +1236,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Roberta_L_Training time</t>
+          <t>RobertaL_Training time</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1260,7 +1260,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Roberta_L_smix_MCC scores</t>
+          <t>RobertaLS_MCC scores</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1284,7 +1284,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Roberta_L_smix_Classification time</t>
+          <t>RobertaLS_Classification time</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1308,7 +1308,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Roberta_L_smix_Training time</t>
+          <t>RobertaLS_Training time</t>
         </is>
       </c>
       <c r="B40" t="n">

</xml_diff>